<commit_message>
实现规范GB50736_2012_6_6_13 GB50736_2012_7_4_13 GB50189_2015_4_2_5 GB50189_2015_4_2_10 GB50189_2015_4_2_14 GB50189_2015_4_2_17 GB50189_2015_4_2_19
</commit_message>
<xml_diff>
--- a/UnitTestHVACChecker/测试数据/测试数据_GB51251_2017_4_4_1.xlsx
+++ b/UnitTestHVACChecker/测试数据/测试数据_GB51251_2017_4_4_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="18260" windowHeight="7080" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="18260" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="风口" sheetId="29" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>楼层编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,22 @@
   </si>
   <si>
     <t>风机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37,38,39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27,28,29,30,31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32,33,34,35,36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27,28,29,30,31,32,33,34,35,36,37,38,39</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -497,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -698,7 +714,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -738,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -758,7 +774,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -778,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -958,7 +974,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -998,7 +1014,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1018,7 +1034,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1038,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1047,6 +1063,266 @@
         <v>0</v>
       </c>
       <c r="F27">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40">
         <v>1000</v>
       </c>
     </row>
@@ -1059,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1108,6 +1384,30 @@
       </c>
       <c r="B5" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1421,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1169,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1230,6 +1530,20 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1241,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>